<commit_message>
added simulations and tets
</commit_message>
<xml_diff>
--- a/scripts/simulation_vision.xlsx
+++ b/scripts/simulation_vision.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eshta\Documents\EB\UofT\Semester 2 - Winter 2023\INF3104\Paper\Final Paper\datasheet_quality_analysis\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C869077D-FB9D-4A8B-8C8D-2B3EB2085F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05371F7-8B72-43C3-9383-7ADF69BC3A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{DEB4D7DA-172A-4198-9636-3923D3C13701}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" activeTab="2" xr2:uid="{DEB4D7DA-172A-4198-9636-3923D3C13701}"/>
   </bookViews>
   <sheets>
     <sheet name="2018" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>q_num</t>
   </si>
@@ -61,9 +61,6 @@
     <t>datasheet_id</t>
   </si>
   <si>
-    <t>title of paper</t>
-  </si>
-  <si>
     <t>shortcut title</t>
   </si>
   <si>
@@ -91,13 +88,13 @@
     <t>max_question_num</t>
   </si>
   <si>
-    <t>top_10_frequent_words_overall</t>
-  </si>
-  <si>
     <t>score</t>
   </si>
   <si>
     <t>datasheet_version</t>
+  </si>
+  <si>
+    <t>top_5_frequent_words_overall</t>
   </si>
 </sst>
 </file>
@@ -451,7 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444BD056-CBEC-4005-A685-424AC9DDFD17}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -465,7 +462,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -774,7 +771,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1102,29 +1099,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EFDA69-6FDF-4566-BBA9-0D97E634BDDC}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="11.31640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.2265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.2265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.2265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5" customWidth="1"/>
-    <col min="10" max="10" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.953125" customWidth="1"/>
-    <col min="13" max="13" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.2265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.2265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.2265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5" customWidth="1"/>
+    <col min="9" max="9" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.953125" customWidth="1"/>
+    <col min="12" max="12" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1147,122 +1144,119 @@
         <v>12</v>
       </c>
       <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
       <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.75">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>2018</v>
+      </c>
       <c r="D2">
-        <v>2018</v>
-      </c>
-      <c r="E2">
         <v>5000</v>
       </c>
+      <c r="F2">
+        <v>300</v>
+      </c>
       <c r="G2">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>3</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>500</v>
       </c>
       <c r="J2">
-        <v>500</v>
-      </c>
-      <c r="K2">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <v>2021</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="C4">
         <v>2021</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>